<commit_message>
Result generated in tables
The result has been generated in tables
</commit_message>
<xml_diff>
--- a/rubricdetail/Rubrics.xlsx
+++ b/rubricdetail/Rubrics.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>Rubric Number</t>
   </si>
@@ -41,13 +41,16 @@
     <t>4</t>
   </si>
   <si>
+    <t>3</t>
+  </si>
+  <si>
     <t>1</t>
   </si>
   <si>
     <t>Discription</t>
   </si>
   <si>
-    <t>3</t>
+    <t>10</t>
   </si>
   <si>
     <t>Level 1 Discription</t>
@@ -141,22 +144,22 @@
         <v>9</v>
       </c>
       <c r="C2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>